<commit_message>
RA and Dec data added
Took RA and Dec data for perhaps half of the GRBs from the Swift website. Antonio and I decided to use the XRT positions instead of BAT ones  to ensure accuracy
</commit_message>
<xml_diff>
--- a/Datalog.xlsx
+++ b/Datalog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Documents/GRB-SNe/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AB3919-5DA3-144A-AAF3-06B582444896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D1528-9104-A744-B60C-F0E809EBB840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5140" yWindow="1740" windowWidth="28040" windowHeight="17440" xr2:uid="{F4B7B060-89A2-5540-85B0-FC3B21031AC9}"/>
   </bookViews>
@@ -401,254 +401,224 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -970,8 +940,8 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1277,7 @@
       <c r="D20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="5" t="s">
         <v>84</v>
       </c>
       <c r="F20" s="4"/>
@@ -1908,6 +1878,7 @@
     <hyperlink ref="E33" r:id="rId4" xr:uid="{2698259A-CE0B-7E41-8C40-62299800F6ED}"/>
     <hyperlink ref="E34" r:id="rId5" xr:uid="{98B4D74C-ED82-6746-AC95-463CFECC9566}"/>
     <hyperlink ref="I23" r:id="rId6" xr:uid="{6C993DC3-940C-374D-9B3B-F4A4D6A829E1}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{ED7EDAEB-BA9C-044C-BD2E-35387EBF203C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>